<commit_message>
feat(checkout): singular item working and written into the cell
</commit_message>
<xml_diff>
--- a/Database/Orders.xlsx
+++ b/Database/Orders.xlsx
@@ -1,51 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Baja Drive\ucalg-baja-cloud\Database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D1776A-4A21-4371-AB96-03F7D7E9FAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1110" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1110" windowWidth="19200" windowHeight="11170"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Order Id</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Item Id</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Size</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Quantity</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>d5531907-1cc6-4abb-8302-5182051301be</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HERO-2020 HOODIES</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>df4b0000-1a5e-4d9a-af8b-73db6ecf3a59</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,14 +91,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -242,15 +248,15 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:lumMod val="102000"/>
                 <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:lumMod val="100000"/>
                 <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
@@ -311,32 +317,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
+            <a:satMod val="170000"/>
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
+                <a:lumMod val="102000"/>
                 <a:satMod val="150000"/>
                 <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
+                <a:lumMod val="103000"/>
                 <a:satMod val="130000"/>
                 <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:satMod val="120000"/>
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -347,23 +353,21 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="5" width="8.38" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -382,7 +386,42 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(merch): accepting json by url path (#1)
</commit_message>
<xml_diff>
--- a/Database/Orders.xlsx
+++ b/Database/Orders.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1110" windowWidth="19200" windowHeight="11170"/>
+    <workbookView activeTab="0" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>d5531907-1cc6-4abb-8302-5182051301be</t>
+    <t>b33c2c8f-d292-43f9-813d-57f0a48e9e5c</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -48,7 +48,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>df4b0000-1a5e-4d9a-af8b-73db6ecf3a59</t>
+    <t>XL</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -56,13 +56,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,7 +79,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -85,8 +98,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,20 +166,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -178,12 +209,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -222,131 +253,152 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:satMod val="300000"/>
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+                <a:tint val="37000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:satMod val="103000"/>
+                <a:satMod val="130000"/>
+                <a:tint val="51000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="130000"/>
+                <a:tint val="15000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="135000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:satMod val="110000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:satMod val="105000"/>
+              <a:shade val="9500"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:satMod val="170000"/>
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:tint val="93000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="103000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:tint val="98000"/>
+                <a:satMod val="350000"/>
+                <a:tint val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="350000"/>
+                <a:shade val="99000"/>
+                <a:tint val="45000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:satMod val="120000"/>
-                <a:shade val="63000"/>
+                <a:satMod val="255000"/>
+                <a:tint val="20000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="200000"/>
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -360,63 +412,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="8.38" customWidth="1"/>
+    <col min="1" max="3" width="8.43357142857143" bestFit="1" customWidth="1" style="1"/>
+    <col min="4" max="4" width="8.43357142857143" bestFit="1" customWidth="1" style="5"/>
+    <col min="5" max="5" width="8.43357142857143" bestFit="1" customWidth="1" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="1">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="1">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>36.0099983215332</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>36.0099983215332</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(recieve orders): wrties customer info to excel sheet (#1)
</commit_message>
<xml_diff>
--- a/Database/Orders.xlsx
+++ b/Database/Orders.xlsx
@@ -4,22 +4,39 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView activeTab="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
+    <sheet name="customer_info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>Order Id</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Email</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Phone</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Subteam</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>Item Id</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -36,7 +53,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>b33c2c8f-d292-43f9-813d-57f0a48e9e5c</t>
+    <t>93616598-94e1-4b54-ae94-ccce8393d8bb</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -49,6 +66,26 @@
   </si>
   <si>
     <t>XL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>brock.tomlinson@ucalgary.ca</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Brock</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Software</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2509466196</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -56,13 +93,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -98,19 +141,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -139,31 +191,31 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="44546a"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="e7e6e6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="5b9bd5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="ed7d31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="a5a5a5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="ffc000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4472c4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="70ad47"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -410,18 +462,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="8.43357142857143" bestFit="1" customWidth="1" style="1"/>
+    <col min="4" max="4" width="8.43357142857143" bestFit="1" customWidth="1" style="8"/>
+    <col min="5" max="5" width="8.43357142857143" bestFit="1" customWidth="1" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s" s="4">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
+      <c r="E6" s="9">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="8">
+        <v>10</v>
+      </c>
+      <c r="E7" s="9">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="9">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="D9" s="8">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9">
+        <v>36.0099983215332</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.43357142857143" bestFit="1" customWidth="1" style="1"/>
-    <col min="4" max="4" width="8.43357142857143" bestFit="1" customWidth="1" style="5"/>
-    <col min="5" max="5" width="8.43357142857143" bestFit="1" customWidth="1" style="6"/>
+    <col min="1" max="5" width="12.43357142857143" bestFit="1" customWidth="1" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
@@ -431,45 +653,45 @@
       <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" t="s" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6">
-        <v>36.0099983215332</v>
+        <v>14</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2509466196</v>
+      </c>
+      <c r="D2" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>36.0099983215332</v>
+        <v>17</v>
+      </c>
+      <c r="D3" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s" s="1">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>